<commit_message>
Deuxieme version de la maquette 	+ Maquette fonctionelle 	+ Ajout de fichiers css et de script pour le menu dropdown
</commit_message>
<xml_diff>
--- a/SEEMULLERJ_TPI_2015/doc/SEEMULLER Julien TPI, Planning journalier.xlsx
+++ b/SEEMULLERJ_TPI_2015/doc/SEEMULLER Julien TPI, Planning journalier.xlsx
@@ -426,7 +426,7 @@
                   <c:v>42122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42122</c:v>
+                  <c:v>42123</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42122</c:v>
@@ -513,10 +513,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,11 +535,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="131152896"/>
-        <c:axId val="124426432"/>
+        <c:axId val="130100224"/>
+        <c:axId val="124491968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131152896"/>
+        <c:axId val="130100224"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -545,7 +548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124426432"/>
+        <c:crossAx val="124491968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,7 +556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124426432"/>
+        <c:axId val="124491968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42139"/>
@@ -566,7 +569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131152896"/>
+        <c:crossAx val="130100224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -917,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,11 +956,11 @@
         <v>42122</v>
       </c>
       <c r="D2" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6">
         <f>C2+D2</f>
-        <v>42124</v>
+        <v>42125</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -980,12 +983,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="5">
-        <v>42122</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>42123</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
       <c r="E4" s="6">
         <f t="shared" si="0"/>
-        <v>42122</v>
+        <v>42125</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>

</xml_diff>

<commit_message>
Mise à jour de la structure des produits, Ajout de la maquette du formulaire d'ajout 	+ Formulaire d'ajout 	+ Structure index.php 	- Suppression de fichiers innutiles
</commit_message>
<xml_diff>
--- a/SEEMULLERJ_TPI_2015/doc/SEEMULLER Julien TPI, Planning journalier.xlsx
+++ b/SEEMULLERJ_TPI_2015/doc/SEEMULLER Julien TPI, Planning journalier.xlsx
@@ -429,13 +429,13 @@
                   <c:v>42123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42122</c:v>
+                  <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>42122</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42122</c:v>
+                  <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>42122</c:v>
@@ -444,7 +444,7 @@
                   <c:v>42122</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42122</c:v>
+                  <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42122</c:v>
@@ -513,13 +513,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,11 +544,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="130100224"/>
-        <c:axId val="124491968"/>
+        <c:axId val="117455872"/>
+        <c:axId val="105027776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130100224"/>
+        <c:axId val="117455872"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -548,7 +557,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124491968"/>
+        <c:crossAx val="105027776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -556,7 +565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124491968"/>
+        <c:axId val="105027776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42139"/>
@@ -569,7 +578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130100224"/>
+        <c:crossAx val="117455872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -920,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,11 +965,11 @@
         <v>42122</v>
       </c>
       <c r="D2" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6">
         <f>C2+D2</f>
-        <v>42125</v>
+        <v>42130</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1000,12 +1009,14 @@
         <v>7</v>
       </c>
       <c r="C5" s="8">
-        <v>42122</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>42124</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
       <c r="E5" s="10">
         <f t="shared" si="0"/>
-        <v>42122</v>
+        <v>42125</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1026,12 +1037,14 @@
         <v>9</v>
       </c>
       <c r="C7" s="8">
-        <v>42122</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>42124</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
       <c r="E7" s="10">
         <f t="shared" ref="E7:E8" si="1">C7+D7</f>
-        <v>42122</v>
+        <v>42129</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1065,12 +1078,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="5">
-        <v>42122</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>42124</v>
+      </c>
+      <c r="D10" s="4">
+        <v>6</v>
+      </c>
       <c r="E10" s="6">
         <f t="shared" ref="E10:E11" si="3">C10+D10</f>
-        <v>42122</v>
+        <v>42130</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ajout de fonctions, Mise à jour documentation 	+ Recherche de produit fonctionnelle 		+ Recherche par mot-clef 		+ Recherche par barre de recherche 	+ Mise à jour planning 	+ Mise à jour base de données
</commit_message>
<xml_diff>
--- a/SEEMULLERJ_TPI_2015/doc/SEEMULLER Julien TPI, Planning journalier.xlsx
+++ b/SEEMULLERJ_TPI_2015/doc/SEEMULLER Julien TPI, Planning journalier.xlsx
@@ -432,22 +432,22 @@
                   <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42122</c:v>
+                  <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42122</c:v>
+                  <c:v>42131</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42122</c:v>
+                  <c:v>42131</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>42124</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42122</c:v>
+                  <c:v>42132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,7 +513,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -524,11 +524,23 @@
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="8">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,11 +556,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="117455872"/>
-        <c:axId val="105027776"/>
+        <c:axId val="117984256"/>
+        <c:axId val="110270656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117455872"/>
+        <c:axId val="117984256"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -557,7 +569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105027776"/>
+        <c:crossAx val="110270656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105027776"/>
+        <c:axId val="110270656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42139"/>
@@ -578,11 +590,18 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117455872"/>
+        <c:crossAx val="117984256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
         <a:scene3d>
           <a:camera prst="orthographicFront"/>
           <a:lightRig rig="threePt" dir="t"/>
@@ -929,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,11 +984,11 @@
         <v>42122</v>
       </c>
       <c r="D2" s="4">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6">
         <f>C2+D2</f>
-        <v>42130</v>
+        <v>42139</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1024,12 +1043,14 @@
         <v>8</v>
       </c>
       <c r="C6" s="5">
-        <v>42122</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>42124</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8</v>
+      </c>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
-        <v>42122</v>
+        <v>42132</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1052,12 +1073,14 @@
         <v>10</v>
       </c>
       <c r="C8" s="5">
-        <v>42122</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>42131</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>42122</v>
+        <v>42132</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1065,12 +1088,14 @@
         <v>11</v>
       </c>
       <c r="C9" s="8">
-        <v>42122</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>42131</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
       <c r="E9" s="10">
         <f t="shared" ref="E9" si="2">C9+D9</f>
-        <v>42122</v>
+        <v>42132</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1093,12 +1118,14 @@
         <v>13</v>
       </c>
       <c r="C11" s="12">
-        <v>42122</v>
-      </c>
-      <c r="D11" s="13"/>
+        <v>42132</v>
+      </c>
+      <c r="D11" s="13">
+        <v>7</v>
+      </c>
       <c r="E11" s="14">
         <f t="shared" si="3"/>
-        <v>42122</v>
+        <v>42139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>